<commit_message>
Finally deleted the todelete file
</commit_message>
<xml_diff>
--- a/data/dataSchemas/databaseIngestSchema.xlsx
+++ b/data/dataSchemas/databaseIngestSchema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/dataSchemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4072C29E-291B-4261-A5A4-2F0AD9F84D19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{4072C29E-291B-4261-A5A4-2F0AD9F84D19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{004C2689-42ED-4898-A5D7-0836A015DA4C}"/>
   <bookViews>
-    <workbookView xWindow="29205" yWindow="-8130" windowWidth="15795" windowHeight="20835" firstSheet="2" activeTab="4" xr2:uid="{494DBC99-8CF9-1C4B-AA75-A6ED73BF8BA1}"/>
+    <workbookView xWindow="7785" yWindow="-3105" windowWidth="12150" windowHeight="20835" firstSheet="5" activeTab="5" xr2:uid="{494DBC99-8CF9-1C4B-AA75-A6ED73BF8BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="chemicalByExtractSample" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1381,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6703CE3-0794-3742-BCAF-B07C34E4436B}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1512,13 +1512,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A982544-BF5A-B341-92AC-6429ED431738}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="1" max="1" width="27.25" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated schemas and tried to build.
</commit_message>
<xml_diff>
--- a/data/dataSchemas/databaseIngestSchema.xlsx
+++ b/data/dataSchemas/databaseIngestSchema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/dataSchemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosl241\OneDrive - PNNL\Documents\GitHub\srpAnalytics\data\dataSchemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4072C29E-291B-4261-A5A4-2F0AD9F84D19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{004C2689-42ED-4898-A5D7-0836A015DA4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CCC4CA-BE57-4CB2-84E7-5F73780651B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7785" yWindow="-3105" windowWidth="12150" windowHeight="20835" firstSheet="5" activeTab="5" xr2:uid="{494DBC99-8CF9-1C4B-AA75-A6ED73BF8BA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="5" xr2:uid="{494DBC99-8CF9-1C4B-AA75-A6ED73BF8BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="chemicalByExtractSample" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="84">
   <si>
     <t>Variable</t>
   </si>
@@ -262,15 +262,52 @@
   </si>
   <si>
     <t>AlternateName</t>
+  </si>
+  <si>
+    <t>Measurement of chemical in M</t>
+  </si>
+  <si>
+    <t>Unit measured</t>
+  </si>
+  <si>
+    <t>Measurement of chemical in water</t>
+  </si>
+  <si>
+    <t>CAS identifier</t>
+  </si>
+  <si>
+    <t>Name of sample</t>
+  </si>
+  <si>
+    <t>Number of sample</t>
+  </si>
+  <si>
+    <t>Internal chemical identifier</t>
+  </si>
+  <si>
+    <t>Internal sample identifier</t>
+  </si>
+  <si>
+    <t>ProjectName</t>
+  </si>
+  <si>
+    <t>ProjectLink</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -291,6 +328,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -300,7 +350,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -308,22 +358,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,19 +731,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9C65D1-6CF8-8C49-A7DB-A6A9CD2A72C5}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="29.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,8 +757,12 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -677,8 +775,11 @@
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -691,8 +792,11 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -705,8 +809,11 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -719,8 +826,11 @@
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -733,8 +843,11 @@
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -747,8 +860,11 @@
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -761,8 +877,11 @@
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -775,8 +894,11 @@
       <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -789,18 +911,31 @@
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="E10" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C1FA9B-D401-F840-B303-06F6F3FDB15F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -809,7 +944,7 @@
     <col min="3" max="3" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -822,8 +957,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -837,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -851,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -865,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -879,7 +1017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -893,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -907,7 +1045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -921,7 +1059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -931,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F71566-F96C-0A49-93E7-C742899FF38D}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -945,7 +1083,7 @@
     <col min="4" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -958,8 +1096,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -973,7 +1114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -987,7 +1128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -1001,7 +1142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1156,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1029,7 +1170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1043,7 +1184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1057,7 +1198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1071,7 +1212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1085,7 +1226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -1099,7 +1240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -1113,7 +1254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
@@ -1127,7 +1268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
@@ -1141,7 +1282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
@@ -1155,7 +1296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -1274,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71543B86-483A-EF4D-9E3F-4D7A5375586B}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1429,7 @@
     <col min="4" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1301,8 +1442,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>56</v>
       </c>
@@ -1330,7 +1474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -1344,7 +1488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1358,7 +1502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1379,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6703CE3-0794-3742-BCAF-B07C34E4436B}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1391,7 +1535,7 @@
     <col min="3" max="3" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1404,8 +1548,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1433,7 +1580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -1447,7 +1594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1461,7 +1608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1475,7 +1622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1510,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A982544-BF5A-B341-92AC-6429ED431738}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1669,7 @@
     <col min="3" max="3" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1535,8 +1682,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -1550,7 +1700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1564,7 +1714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -1578,7 +1728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1592,7 +1742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1606,7 +1756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -1620,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>62</v>
       </c>
@@ -1648,7 +1798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>65</v>
       </c>
@@ -1662,7 +1812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>66</v>
       </c>
@@ -1676,7 +1826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1690,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>67</v>
       </c>
@@ -1704,7 +1854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1718,7 +1868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>68</v>
       </c>
@@ -1732,7 +1882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>70</v>
       </c>
@@ -1841,6 +1991,34 @@
         <v>54</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1851,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41185C6F-4B94-4C48-A72F-1F634AE26AAD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1865,7 +2043,7 @@
     <col min="4" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1878,8 +2056,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1893,7 +2074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>56</v>
       </c>
@@ -1907,7 +2088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -1921,7 +2102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1935,7 +2116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>